<commit_message>
fixed one more issue in FA.py
</commit_message>
<xml_diff>
--- a/Python/output/case-study/FC_SA_FAresults-KPI.xlsx
+++ b/Python/output/case-study/FC_SA_FAresults-KPI.xlsx
@@ -1,28 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27715"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/local_ysong3/Documents/GitHub/msp_models_for_adaptive_disaster_relief_logistics_planning/Python/output/case-study/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yongjis/Desktop/temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CF7C850A-F756-8E41-A5CC-3D5E9D981D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="3600" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="9680" yWindow="7140" windowWidth="27640" windowHeight="16940" xr2:uid="{D4483AFD-FD69-D349-8C68-591E446E8457}"/>
   </bookViews>
   <sheets>
     <sheet name="FC_SA_FAresults-KPI" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -62,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -540,8 +533,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -916,11 +910,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6674B712-5FB8-3C4D-9F6D-224560BCBEFA}">
   <dimension ref="A1:BB11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -980,13 +974,13 @@
         <v>8500</v>
       </c>
       <c r="H2">
-        <v>8149.5637340053299</v>
+        <v>8154.2815454090396</v>
       </c>
       <c r="I2">
-        <v>7418.2404459217396</v>
+        <v>7400.5319544003996</v>
       </c>
       <c r="J2">
-        <v>6473.3635219301505</v>
+        <v>6472.8673395946598</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1016,7 +1010,7 @@
         <v>0.88200000000000001</v>
       </c>
       <c r="T2">
-        <v>0.79900000000000004</v>
+        <v>0.79100000000000004</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1040,13 +1034,13 @@
         <v>8500</v>
       </c>
       <c r="AB2">
-        <v>8315.8813612299291</v>
+        <v>8320.6954544990203</v>
       </c>
       <c r="AC2">
-        <v>8410.7034534260092</v>
+        <v>8390.6257986399105</v>
       </c>
       <c r="AD2">
-        <v>8101.8316920277302</v>
+        <v>8183.1445506885702</v>
       </c>
       <c r="AE2">
         <v>0</v>
@@ -1073,10 +1067,10 @@
         <v>0</v>
       </c>
       <c r="AM2">
-        <v>7.5169028267302096</v>
+        <v>1.12509774144034</v>
       </c>
       <c r="AN2">
-        <v>30.616446383486998</v>
+        <v>32.574527050575703</v>
       </c>
       <c r="AO2">
         <v>0</v>
@@ -1088,13 +1082,13 @@
         <v>0</v>
       </c>
       <c r="AR2">
-        <v>46034.591961944701</v>
+        <v>56027.680839403802</v>
       </c>
       <c r="AS2">
-        <v>32376.063319928999</v>
+        <v>32336.716786871599</v>
       </c>
       <c r="AT2">
-        <v>3928.6441246755498</v>
+        <v>3902.78445407138</v>
       </c>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.2">
@@ -1114,19 +1108,19 @@
         <v>8313</v>
       </c>
       <c r="F3">
-        <v>11180.036382865401</v>
+        <v>11326.4726206172</v>
       </c>
       <c r="G3">
-        <v>14718.112689759</v>
+        <v>14663.4798708008</v>
       </c>
       <c r="H3">
-        <v>13073.435939484099</v>
+        <v>13012.069577864901</v>
       </c>
       <c r="I3">
-        <v>11390.590259762201</v>
+        <v>11376.010270058399</v>
       </c>
       <c r="J3">
-        <v>8773.6730921966591</v>
+        <v>8899.7322322024793</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1150,13 +1144,13 @@
         <v>0.98799999999999999</v>
       </c>
       <c r="R3">
-        <v>0.91300000000000003</v>
+        <v>0.91</v>
       </c>
       <c r="S3">
-        <v>0.76500000000000001</v>
+        <v>0.754</v>
       </c>
       <c r="T3">
-        <v>0.64300000000000002</v>
+        <v>0.629</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1174,19 +1168,19 @@
         <v>17000</v>
       </c>
       <c r="Z3">
-        <v>11793.287323697699</v>
+        <v>11947.7559289211</v>
       </c>
       <c r="AA3">
-        <v>14896.875192063801</v>
+        <v>14841.5788166</v>
       </c>
       <c r="AB3">
-        <v>14319.2069435751</v>
+        <v>14298.9775580934</v>
       </c>
       <c r="AC3">
-        <v>14889.6604702774</v>
+        <v>15087.546777265799</v>
       </c>
       <c r="AD3">
-        <v>13644.903720368</v>
+        <v>14149.017830876701</v>
       </c>
       <c r="AE3">
         <v>0</v>
@@ -1212,11 +1206,11 @@
       <c r="AL3">
         <v>0</v>
       </c>
-      <c r="AM3">
-        <v>0</v>
+      <c r="AM3" s="1">
+        <v>-5.09201443868273E-11</v>
       </c>
       <c r="AN3">
-        <v>68.280989193914394</v>
+        <v>119.49138225761</v>
       </c>
       <c r="AO3">
         <v>0</v>
@@ -1228,13 +1222,13 @@
         <v>0</v>
       </c>
       <c r="AR3">
-        <v>61266.131892091798</v>
+        <v>84590.764571542706</v>
       </c>
       <c r="AS3">
-        <v>57377.450618982599</v>
+        <v>57457.690723968197</v>
       </c>
       <c r="AT3">
-        <v>522.35076151900103</v>
+        <v>460.67465902816002</v>
       </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.2">
@@ -1257,16 +1251,16 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>14503.349395454599</v>
+        <v>14644.6858046045</v>
       </c>
       <c r="H4">
-        <v>27115.793171804002</v>
+        <v>27407.792237613001</v>
       </c>
       <c r="I4">
-        <v>23447.207425557499</v>
+        <v>23766.275375901299</v>
       </c>
       <c r="J4">
-        <v>19343.280036453401</v>
+        <v>19277.522172099401</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1290,13 +1284,13 @@
         <v>0.63300000000000001</v>
       </c>
       <c r="R4">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="S4">
-        <v>0.92200000000000004</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="T4">
-        <v>0.83499999999999996</v>
+        <v>0.80900000000000005</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -1317,16 +1311,16 @@
         <v>0</v>
       </c>
       <c r="AA4">
-        <v>22912.084353008901</v>
+        <v>23135.364620228302</v>
       </c>
       <c r="AB4">
-        <v>27669.176705922499</v>
+        <v>27407.792237613001</v>
       </c>
       <c r="AC4">
-        <v>25430.8106567869</v>
+        <v>25974.0714490725</v>
       </c>
       <c r="AD4">
-        <v>23165.604761107101</v>
+        <v>23828.828395672899</v>
       </c>
       <c r="AE4">
         <v>0</v>
@@ -1350,13 +1344,13 @@
         <v>0</v>
       </c>
       <c r="AL4">
-        <v>0</v>
+        <v>29.939842693673999</v>
       </c>
       <c r="AM4">
-        <v>0</v>
+        <v>1.4722042540484901</v>
       </c>
       <c r="AN4">
-        <v>36.1214598295348</v>
+        <v>32.395950729590403</v>
       </c>
       <c r="AO4">
         <v>0</v>
@@ -1368,13 +1362,13 @@
         <v>0</v>
       </c>
       <c r="AR4">
-        <v>62237.1473834629</v>
+        <v>85096.275590217905</v>
       </c>
       <c r="AS4">
-        <v>57167.626047763297</v>
+        <v>57777.725226495997</v>
       </c>
       <c r="AT4">
-        <v>351.74452509743298</v>
+        <v>275.19814288144102</v>
       </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.2">
@@ -1400,13 +1394,13 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1181.8343468875601</v>
+        <v>1261.5817570340701</v>
       </c>
       <c r="I5">
-        <v>38595.234080894101</v>
+        <v>38898.224162028899</v>
       </c>
       <c r="J5">
-        <v>44864.463157549697</v>
+        <v>45277.336026757002</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -1430,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>0.1</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="S5">
         <v>0.92100000000000004</v>
@@ -1460,13 +1454,13 @@
         <v>0</v>
       </c>
       <c r="AB5">
-        <v>11818.343468875601</v>
+        <v>14175.075921731101</v>
       </c>
       <c r="AC5">
-        <v>41905.791618777599</v>
+        <v>42234.771077121499</v>
       </c>
       <c r="AD5">
-        <v>45044.641724447501</v>
+        <v>45459.172717627502</v>
       </c>
       <c r="AE5">
         <v>0</v>
@@ -1496,7 +1490,7 @@
         <v>0</v>
       </c>
       <c r="AN5">
-        <v>12.915413250047701</v>
+        <v>11.9152096590337</v>
       </c>
       <c r="AO5">
         <v>0</v>
@@ -1508,13 +1502,13 @@
         <v>0</v>
       </c>
       <c r="AR5">
-        <v>62646.286689665103</v>
+        <v>85437.141945819996</v>
       </c>
       <c r="AS5">
-        <v>57357.635333168597</v>
+        <v>58071.311870656202</v>
       </c>
       <c r="AT5">
-        <v>309.852254440693</v>
+        <v>227.91843144007899</v>
       </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.2">
@@ -1543,10 +1537,10 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>1590.10729400839</v>
+        <v>1697.19438186918</v>
       </c>
       <c r="J6">
-        <v>83326.894410233101</v>
+        <v>83877.858197528796</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1603,10 +1597,10 @@
         <v>0</v>
       </c>
       <c r="AC6">
-        <v>12520.5298740818</v>
+        <v>13363.735290308499</v>
       </c>
       <c r="AD6">
-        <v>83326.894410233101</v>
+        <v>83877.858197528796</v>
       </c>
       <c r="AE6">
         <v>0</v>
@@ -1638,8 +1632,8 @@
       <c r="AN6">
         <v>0</v>
       </c>
-      <c r="AO6">
-        <v>0</v>
+      <c r="AO6" s="1">
+        <v>-9.9015242107961194E-12</v>
       </c>
       <c r="AP6">
         <v>0</v>
@@ -1648,13 +1642,13 @@
         <v>0</v>
       </c>
       <c r="AR6">
-        <v>62842.950181874003</v>
+        <v>85575.052579397801</v>
       </c>
       <c r="AS6">
-        <v>57633.112655817</v>
+        <v>58208.288070174298</v>
       </c>
       <c r="AT6">
-        <v>309.85945817948499</v>
+        <v>226.983997380397</v>
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.2">
@@ -1683,16 +1677,16 @@
         <v>8500</v>
       </c>
       <c r="I7">
-        <v>8345.59537121619</v>
+        <v>8440.2726089314292</v>
       </c>
       <c r="J7">
-        <v>7692.3299047097598</v>
+        <v>7669.6124676230702</v>
       </c>
       <c r="K7">
-        <v>6022.8874896212901</v>
+        <v>6033.4680703964304</v>
       </c>
       <c r="L7">
-        <v>4787.8237946785603</v>
+        <v>5285.2499198350197</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1728,7 +1722,7 @@
         <v>0.82699999999999996</v>
       </c>
       <c r="X7">
-        <v>0.60599999999999998</v>
+        <v>0.68</v>
       </c>
       <c r="Y7">
         <v>0</v>
@@ -1755,16 +1749,16 @@
         <v>8500</v>
       </c>
       <c r="AG7">
-        <v>8345.59537121619</v>
+        <v>8440.2726089314292</v>
       </c>
       <c r="AH7">
-        <v>8114.2720513816103</v>
+        <v>8090.3085101509196</v>
       </c>
       <c r="AI7">
-        <v>7282.8143768092996</v>
+        <v>7295.6082899705098</v>
       </c>
       <c r="AJ7">
-        <v>7900.6993311523502</v>
+        <v>7772.4263526985396</v>
       </c>
       <c r="AK7">
         <v>0</v>
@@ -1797,10 +1791,10 @@
         <v>0</v>
       </c>
       <c r="AU7">
-        <v>0</v>
+        <v>1.05473173441434E-3</v>
       </c>
       <c r="AV7">
-        <v>49.642128232664099</v>
+        <v>32.798839934460602</v>
       </c>
       <c r="AW7">
         <v>0</v>
@@ -1812,13 +1806,13 @@
         <v>0</v>
       </c>
       <c r="AZ7">
-        <v>52297.820974880698</v>
+        <v>69928.603066785698</v>
       </c>
       <c r="BA7">
-        <v>47697.650379976098</v>
+        <v>48163.570247952499</v>
       </c>
       <c r="BB7">
-        <v>2207.4983216995302</v>
+        <v>2093.4516831158498</v>
       </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.2">
@@ -1838,25 +1832,25 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>4379.09952417766</v>
+        <v>4378.8265096777304</v>
       </c>
       <c r="G8">
-        <v>16999.789716754702</v>
+        <v>16999.999994273701</v>
       </c>
       <c r="H8">
-        <v>16991.8582220389</v>
+        <v>16999.999999999902</v>
       </c>
       <c r="I8">
-        <v>16073.4592501478</v>
+        <v>16313.7494493782</v>
       </c>
       <c r="J8">
-        <v>13326.340905254499</v>
+        <v>12849.7353790417</v>
       </c>
       <c r="K8">
-        <v>9954.8559547574205</v>
+        <v>10019.667892981601</v>
       </c>
       <c r="L8">
-        <v>7291.3161683007502</v>
+        <v>7506.8230838366098</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1886,13 +1880,13 @@
         <v>1</v>
       </c>
       <c r="V8">
-        <v>0.88600000000000001</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="W8">
-        <v>0.71599999999999997</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="X8">
-        <v>0.56499999999999995</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="Y8">
         <v>0</v>
@@ -1910,25 +1904,25 @@
         <v>0</v>
       </c>
       <c r="AD8">
-        <v>4379.09952417766</v>
+        <v>4378.8265096777304</v>
       </c>
       <c r="AE8">
-        <v>16999.789716754702</v>
+        <v>16999.999994273701</v>
       </c>
       <c r="AF8">
-        <v>16991.8582220389</v>
+        <v>16999.999999999902</v>
       </c>
       <c r="AG8">
-        <v>16073.4592501478</v>
+        <v>16313.7494493782</v>
       </c>
       <c r="AH8">
-        <v>15041.0168230864</v>
+        <v>14043.426643761401</v>
       </c>
       <c r="AI8">
-        <v>13903.430104409799</v>
+        <v>13974.432207784699</v>
       </c>
       <c r="AJ8">
-        <v>12904.9843686738</v>
+        <v>12346.748493152299</v>
       </c>
       <c r="AK8">
         <v>0</v>
@@ -1957,14 +1951,14 @@
       <c r="AS8">
         <v>0</v>
       </c>
-      <c r="AT8">
-        <v>0</v>
-      </c>
-      <c r="AU8">
-        <v>0</v>
+      <c r="AT8" s="1">
+        <v>-3.4327285982361501E-11</v>
+      </c>
+      <c r="AU8" s="1">
+        <v>-1.3295010858928701E-10</v>
       </c>
       <c r="AV8">
-        <v>69.269329771324607</v>
+        <v>46.489712965007598</v>
       </c>
       <c r="AW8">
         <v>0</v>
@@ -1976,13 +1970,13 @@
         <v>0</v>
       </c>
       <c r="AZ8">
-        <v>57976.811749616303</v>
+        <v>85068.802309189399</v>
       </c>
       <c r="BA8">
-        <v>61707.246751240898</v>
+        <v>61589.603311129002</v>
       </c>
       <c r="BB8">
-        <v>549.01151175822997</v>
+        <v>379.28550388842598</v>
       </c>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.2">
@@ -2008,19 +2002,19 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>144.15577124805901</v>
+        <v>348.574876358783</v>
       </c>
       <c r="I9">
-        <v>6100.4333012787602</v>
+        <v>5958.6700849487697</v>
       </c>
       <c r="J9">
-        <v>30460.2564201649</v>
+        <v>30565.014191755901</v>
       </c>
       <c r="K9">
-        <v>25346.824533468</v>
+        <v>25217.5469133732</v>
       </c>
       <c r="L9">
-        <v>17656.829102971999</v>
+        <v>18557.016376922598</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -2053,10 +2047,10 @@
         <v>0.998</v>
       </c>
       <c r="W9">
-        <v>0.93200000000000005</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="X9">
-        <v>0.78</v>
+        <v>0.79900000000000004</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -2080,19 +2074,19 @@
         <v>0</v>
       </c>
       <c r="AF9">
-        <v>7207.7885624029896</v>
+        <v>17428.743817939099</v>
       </c>
       <c r="AG9">
-        <v>6118.7896702896296</v>
+        <v>5976.5998846025796</v>
       </c>
       <c r="AH9">
-        <v>30521.299018201302</v>
+        <v>30626.2667252063</v>
       </c>
       <c r="AI9">
-        <v>27196.163662519299</v>
+        <v>26628.877416444899</v>
       </c>
       <c r="AJ9">
-        <v>22636.960388425599</v>
+        <v>23225.302098776701</v>
       </c>
       <c r="AK9">
         <v>0</v>
@@ -2124,14 +2118,14 @@
       <c r="AT9">
         <v>0</v>
       </c>
-      <c r="AU9">
-        <v>0</v>
+      <c r="AU9" s="1">
+        <v>-3.1338774934949201E-12</v>
       </c>
       <c r="AV9">
-        <v>21.525842183551099</v>
-      </c>
-      <c r="AW9">
-        <v>0</v>
+        <v>10.788178300779</v>
+      </c>
+      <c r="AW9" s="1">
+        <v>-2.48717004138803E-14</v>
       </c>
       <c r="AX9">
         <v>0</v>
@@ -2140,13 +2134,13 @@
         <v>0</v>
       </c>
       <c r="AZ9">
-        <v>57112.915270917998</v>
+        <v>80646.822443359095</v>
       </c>
       <c r="BA9">
-        <v>56454.975324331201</v>
+        <v>57222.045606976899</v>
       </c>
       <c r="BB9">
-        <v>604.96069714873897</v>
+        <v>433.707665566819</v>
       </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.2">
@@ -2178,13 +2172,13 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1333.3172932366001</v>
+        <v>1415.3489355500001</v>
       </c>
       <c r="K10">
-        <v>35555.210237666099</v>
+        <v>36630.801228460499</v>
       </c>
       <c r="L10">
-        <v>41860.369985758101</v>
+        <v>42151.866527651298</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -2250,13 +2244,13 @@
         <v>0</v>
       </c>
       <c r="AH10">
-        <v>27210.557004828599</v>
+        <v>28884.6721540818</v>
       </c>
       <c r="AI10">
-        <v>38858.153265208799</v>
+        <v>40033.662544765597</v>
       </c>
       <c r="AJ10">
-        <v>43244.1838695849</v>
+        <v>43545.316660796801</v>
       </c>
       <c r="AK10">
         <v>0</v>
@@ -2288,11 +2282,11 @@
       <c r="AT10">
         <v>0</v>
       </c>
-      <c r="AU10">
-        <v>0</v>
+      <c r="AU10" s="1">
+        <v>-4.8547826777381104E-12</v>
       </c>
       <c r="AV10">
-        <v>0.60181515082495696</v>
+        <v>10.667175412020301</v>
       </c>
       <c r="AW10">
         <v>0</v>
@@ -2304,13 +2298,13 @@
         <v>0</v>
       </c>
       <c r="AZ10">
-        <v>57159.020358289403</v>
+        <v>80198.016691661993</v>
       </c>
       <c r="BA10">
-        <v>55472.214313980498</v>
+        <v>56738.276479994602</v>
       </c>
       <c r="BB10">
-        <v>581.80129926890004</v>
+        <v>398.74429028173699</v>
       </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.2">
@@ -2345,10 +2339,10 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>2379.82725300744</v>
+        <v>2324.0690372592198</v>
       </c>
       <c r="L11">
-        <v>76361.399349953601</v>
+        <v>77889.032402131794</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -2417,10 +2411,10 @@
         <v>0</v>
       </c>
       <c r="AI11">
-        <v>29022.283573261499</v>
+        <v>28342.3053324295</v>
       </c>
       <c r="AJ11">
-        <v>76361.399349953601</v>
+        <v>77889.032402131794</v>
       </c>
       <c r="AK11">
         <v>0</v>
@@ -2455,26 +2449,26 @@
       <c r="AU11">
         <v>0</v>
       </c>
-      <c r="AV11">
-        <v>0</v>
-      </c>
-      <c r="AW11">
-        <v>0</v>
-      </c>
-      <c r="AX11">
-        <v>0</v>
+      <c r="AV11" s="1">
+        <v>8.8424506117368198E-11</v>
+      </c>
+      <c r="AW11" s="1">
+        <v>-2.0527847732359801E-11</v>
+      </c>
+      <c r="AX11" s="1">
+        <v>-6.4184633888901396E-14</v>
       </c>
       <c r="AY11">
         <v>0</v>
       </c>
       <c r="AZ11">
-        <v>57205.021087191402</v>
+        <v>80213.101439390899</v>
       </c>
       <c r="BA11">
-        <v>55444.870213932903</v>
+        <v>56738.259512596902</v>
       </c>
       <c r="BB11">
-        <v>562.12811292091499</v>
+        <v>383.64257515503601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A bunch of results for the case study are updated
</commit_message>
<xml_diff>
--- a/Python/output/case-study/FC_SA_FAresults-KPI.xlsx
+++ b/Python/output/case-study/FC_SA_FAresults-KPI.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27715"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yongjis/Desktop/temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/local_ysong3/Documents/GitHub/msp_models_for_adaptive_disaster_relief_logistics_planning/Python/output/case-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CF7C850A-F756-8E41-A5CC-3D5E9D981D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9680" yWindow="7140" windowWidth="27640" windowHeight="16940" xr2:uid="{D4483AFD-FD69-D349-8C68-591E446E8457}"/>
+    <workbookView xWindow="15060" yWindow="10300" windowWidth="27640" windowHeight="16940"/>
   </bookViews>
   <sheets>
     <sheet name="FC_SA_FAresults-KPI" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -55,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -910,11 +917,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6674B712-5FB8-3C4D-9F6D-224560BCBEFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,13 +981,13 @@
         <v>8500</v>
       </c>
       <c r="H2">
-        <v>8154.2815454090396</v>
+        <v>8150.0704200518003</v>
       </c>
       <c r="I2">
-        <v>7400.5319544003996</v>
+        <v>7400.5411534089699</v>
       </c>
       <c r="J2">
-        <v>6472.8673395946598</v>
+        <v>6473.3609008049798</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1034,13 +1041,13 @@
         <v>8500</v>
       </c>
       <c r="AB2">
-        <v>8320.6954544990203</v>
+        <v>8316.3983878079598</v>
       </c>
       <c r="AC2">
-        <v>8390.6257986399105</v>
+        <v>8390.6362283548497</v>
       </c>
       <c r="AD2">
-        <v>8183.1445506885702</v>
+        <v>8183.7685218773504</v>
       </c>
       <c r="AE2">
         <v>0</v>
@@ -1067,10 +1074,10 @@
         <v>0</v>
       </c>
       <c r="AM2">
-        <v>1.12509774144034</v>
+        <v>1.1250977419955099</v>
       </c>
       <c r="AN2">
-        <v>32.574527050575703</v>
+        <v>32.6586752295228</v>
       </c>
       <c r="AO2">
         <v>0</v>
@@ -1082,13 +1089,13 @@
         <v>0</v>
       </c>
       <c r="AR2">
-        <v>56027.680839403802</v>
+        <v>56023.972474265604</v>
       </c>
       <c r="AS2">
-        <v>32336.716786871599</v>
+        <v>32333.204041784898</v>
       </c>
       <c r="AT2">
-        <v>3902.78445407138</v>
+        <v>3902.9800741229501</v>
       </c>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.2">
@@ -1108,19 +1115,19 @@
         <v>8313</v>
       </c>
       <c r="F3">
-        <v>11326.4726206172</v>
+        <v>11374.1803313611</v>
       </c>
       <c r="G3">
-        <v>14663.4798708008</v>
+        <v>14631.2853286749</v>
       </c>
       <c r="H3">
-        <v>13012.069577864901</v>
+        <v>12997.503750198601</v>
       </c>
       <c r="I3">
-        <v>11376.010270058399</v>
+        <v>11374.3598271231</v>
       </c>
       <c r="J3">
-        <v>8899.7322322024793</v>
+        <v>8892.5799839159008</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1141,16 +1148,16 @@
         <v>0.94799999999999995</v>
       </c>
       <c r="Q3">
-        <v>0.98799999999999999</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>0.91</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="S3">
-        <v>0.754</v>
+        <v>0.755</v>
       </c>
       <c r="T3">
-        <v>0.629</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1168,19 +1175,19 @@
         <v>17000</v>
       </c>
       <c r="Z3">
-        <v>11947.7559289211</v>
+        <v>11998.0805183134</v>
       </c>
       <c r="AA3">
-        <v>14841.5788166</v>
+        <v>14631.2853286749</v>
       </c>
       <c r="AB3">
-        <v>14298.9775580934</v>
+        <v>14204.922131364599</v>
       </c>
       <c r="AC3">
-        <v>15087.546777265799</v>
+        <v>15065.377254467699</v>
       </c>
       <c r="AD3">
-        <v>14149.017830876701</v>
+        <v>14070.537912056199</v>
       </c>
       <c r="AE3">
         <v>0</v>
@@ -1207,10 +1214,10 @@
         <v>0</v>
       </c>
       <c r="AM3" s="1">
-        <v>-5.09201443868273E-11</v>
+        <v>7.70167958486163E-13</v>
       </c>
       <c r="AN3">
-        <v>119.49138225761</v>
+        <v>130.070431977254</v>
       </c>
       <c r="AO3">
         <v>0</v>
@@ -1222,13 +1229,13 @@
         <v>0</v>
       </c>
       <c r="AR3">
-        <v>84590.764571542706</v>
+        <v>84582.909221272799</v>
       </c>
       <c r="AS3">
-        <v>57457.690723968197</v>
+        <v>57449.8073820848</v>
       </c>
       <c r="AT3">
-        <v>460.67465902816002</v>
+        <v>460.646667415038</v>
       </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.2">
@@ -1251,16 +1258,16 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>14644.6858046045</v>
+        <v>14632.6487718975</v>
       </c>
       <c r="H4">
-        <v>27407.792237613001</v>
+        <v>27436.348027577002</v>
       </c>
       <c r="I4">
-        <v>23766.275375901299</v>
+        <v>23783.9556423457</v>
       </c>
       <c r="J4">
-        <v>19277.522172099401</v>
+        <v>19251.780761506499</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1287,10 +1294,10 @@
         <v>1</v>
       </c>
       <c r="S4">
-        <v>0.91500000000000004</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="T4">
-        <v>0.80900000000000005</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -1311,16 +1318,16 @@
         <v>0</v>
       </c>
       <c r="AA4">
-        <v>23135.364620228302</v>
+        <v>23116.348770770201</v>
       </c>
       <c r="AB4">
-        <v>27407.792237613001</v>
+        <v>27436.348027577002</v>
       </c>
       <c r="AC4">
-        <v>25974.0714490725</v>
+        <v>25936.7019000498</v>
       </c>
       <c r="AD4">
-        <v>23828.828395672899</v>
+        <v>23826.461338498098</v>
       </c>
       <c r="AE4">
         <v>0</v>
@@ -1344,13 +1351,13 @@
         <v>0</v>
       </c>
       <c r="AL4">
-        <v>29.939842693673999</v>
+        <v>0</v>
       </c>
       <c r="AM4">
-        <v>1.4722042540484901</v>
+        <v>0</v>
       </c>
       <c r="AN4">
-        <v>32.395950729590403</v>
+        <v>23.992015566669501</v>
       </c>
       <c r="AO4">
         <v>0</v>
@@ -1362,13 +1369,13 @@
         <v>0</v>
       </c>
       <c r="AR4">
-        <v>85096.275590217905</v>
+        <v>85104.733203326701</v>
       </c>
       <c r="AS4">
-        <v>57777.725226495997</v>
+        <v>57788.213950614001</v>
       </c>
       <c r="AT4">
-        <v>275.19814288144102</v>
+        <v>277.22925389091398</v>
       </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.2">
@@ -1394,13 +1401,13 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1261.5817570340701</v>
+        <v>1221.6869502422001</v>
       </c>
       <c r="I5">
-        <v>38898.224162028899</v>
+        <v>38882.7580529392</v>
       </c>
       <c r="J5">
-        <v>45277.336026757002</v>
+        <v>45193.622994310099</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -1430,7 +1437,7 @@
         <v>0.92100000000000004</v>
       </c>
       <c r="T5">
-        <v>0.996</v>
+        <v>0.998</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -1454,13 +1461,13 @@
         <v>0</v>
       </c>
       <c r="AB5">
-        <v>14175.075921731101</v>
+        <v>13726.819665642701</v>
       </c>
       <c r="AC5">
-        <v>42234.771077121499</v>
+        <v>42217.978341953502</v>
       </c>
       <c r="AD5">
-        <v>45459.172717627502</v>
+        <v>45284.1913770643</v>
       </c>
       <c r="AE5">
         <v>0</v>
@@ -1489,11 +1496,11 @@
       <c r="AM5">
         <v>0</v>
       </c>
-      <c r="AN5">
-        <v>11.9152096590337</v>
-      </c>
-      <c r="AO5">
-        <v>0</v>
+      <c r="AN5" s="1">
+        <v>1.1757081824619299E-6</v>
+      </c>
+      <c r="AO5" s="1">
+        <v>-2.8950539600761901E-12</v>
       </c>
       <c r="AP5">
         <v>0</v>
@@ -1502,13 +1509,13 @@
         <v>0</v>
       </c>
       <c r="AR5">
-        <v>85437.141945819996</v>
+        <v>85298.067997491802</v>
       </c>
       <c r="AS5">
-        <v>58071.311870656202</v>
+        <v>57931.303305896203</v>
       </c>
       <c r="AT5">
-        <v>227.91843144007899</v>
+        <v>226.98381500830499</v>
       </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.2">
@@ -1537,10 +1544,10 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>1697.19438186918</v>
+        <v>1781.60096455194</v>
       </c>
       <c r="J6">
-        <v>83877.858197528796</v>
+        <v>83811.460958038806</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1597,10 +1604,10 @@
         <v>0</v>
       </c>
       <c r="AC6">
-        <v>13363.735290308499</v>
+        <v>14028.3540515901</v>
       </c>
       <c r="AD6">
-        <v>83877.858197528796</v>
+        <v>83811.460958038806</v>
       </c>
       <c r="AE6">
         <v>0</v>
@@ -1632,8 +1639,8 @@
       <c r="AN6">
         <v>0</v>
       </c>
-      <c r="AO6" s="1">
-        <v>-9.9015242107961194E-12</v>
+      <c r="AO6">
+        <v>0</v>
       </c>
       <c r="AP6">
         <v>0</v>
@@ -1642,13 +1649,13 @@
         <v>0</v>
       </c>
       <c r="AR6">
-        <v>85575.052579397801</v>
+        <v>85593.061922590699</v>
       </c>
       <c r="AS6">
-        <v>58208.288070174298</v>
+        <v>58224.340284935402</v>
       </c>
       <c r="AT6">
-        <v>226.983997380397</v>
+        <v>225.02686894876501</v>
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.2">
@@ -1677,16 +1684,16 @@
         <v>8500</v>
       </c>
       <c r="I7">
-        <v>8440.2726089314292</v>
+        <v>8441.6118179445803</v>
       </c>
       <c r="J7">
-        <v>7669.6124676230702</v>
+        <v>7669.3089259242397</v>
       </c>
       <c r="K7">
-        <v>6033.4680703964304</v>
+        <v>6033.2378625561596</v>
       </c>
       <c r="L7">
-        <v>5285.2499198350197</v>
+        <v>5285.2230851219301</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1716,13 +1723,13 @@
         <v>1</v>
       </c>
       <c r="V7">
-        <v>0.94799999999999995</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="W7">
         <v>0.82699999999999996</v>
       </c>
       <c r="X7">
-        <v>0.68</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="Y7">
         <v>0</v>
@@ -1749,16 +1756,16 @@
         <v>8500</v>
       </c>
       <c r="AG7">
-        <v>8440.2726089314292</v>
+        <v>8441.6118179445803</v>
       </c>
       <c r="AH7">
-        <v>8090.3085101509196</v>
+        <v>8141.5169062053601</v>
       </c>
       <c r="AI7">
-        <v>7295.6082899705098</v>
+        <v>7295.3299426313897</v>
       </c>
       <c r="AJ7">
-        <v>7772.4263526985396</v>
+        <v>7783.8337041560399</v>
       </c>
       <c r="AK7">
         <v>0</v>
@@ -1790,11 +1797,11 @@
       <c r="AT7">
         <v>0</v>
       </c>
-      <c r="AU7">
-        <v>1.05473173441434E-3</v>
+      <c r="AU7" s="1">
+        <v>-2.1827872842550201E-13</v>
       </c>
       <c r="AV7">
-        <v>32.798839934460602</v>
+        <v>32.776565429385698</v>
       </c>
       <c r="AW7">
         <v>0</v>
@@ -1806,13 +1813,13 @@
         <v>0</v>
       </c>
       <c r="AZ7">
-        <v>69928.603066785698</v>
+        <v>69929.381691546805</v>
       </c>
       <c r="BA7">
-        <v>48163.570247952499</v>
+        <v>48164.348875568998</v>
       </c>
       <c r="BB7">
-        <v>2093.4516831158498</v>
+        <v>2093.4516859713899</v>
       </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.2">
@@ -1832,25 +1839,25 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>4378.8265096777304</v>
+        <v>4378.8272603183304</v>
       </c>
       <c r="G8">
-        <v>16999.999994273701</v>
+        <v>17000.0000001515</v>
       </c>
       <c r="H8">
-        <v>16999.999999999902</v>
+        <v>17000.0000000418</v>
       </c>
       <c r="I8">
-        <v>16313.7494493782</v>
+        <v>16252.000000067001</v>
       </c>
       <c r="J8">
-        <v>12849.7353790417</v>
+        <v>12867.894606718701</v>
       </c>
       <c r="K8">
-        <v>10019.667892981601</v>
+        <v>10046.869849397801</v>
       </c>
       <c r="L8">
-        <v>7506.8230838366098</v>
+        <v>7510.91411516469</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1877,16 +1884,16 @@
         <v>1</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="V8">
         <v>0.91500000000000004</v>
       </c>
       <c r="W8">
-        <v>0.71699999999999997</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="X8">
-        <v>0.60799999999999998</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="Y8">
         <v>0</v>
@@ -1904,25 +1911,25 @@
         <v>0</v>
       </c>
       <c r="AD8">
-        <v>4378.8265096777304</v>
+        <v>4378.8272603183304</v>
       </c>
       <c r="AE8">
-        <v>16999.999994273701</v>
+        <v>17000.0000001515</v>
       </c>
       <c r="AF8">
-        <v>16999.999999999902</v>
+        <v>17000.0000000418</v>
       </c>
       <c r="AG8">
-        <v>16313.7494493782</v>
+        <v>17000.000000004798</v>
       </c>
       <c r="AH8">
-        <v>14043.426643761401</v>
+        <v>14063.2727942281</v>
       </c>
       <c r="AI8">
-        <v>13974.432207784699</v>
+        <v>13800.6453975245</v>
       </c>
       <c r="AJ8">
-        <v>12346.748493152299</v>
+        <v>12252.714706630801</v>
       </c>
       <c r="AK8">
         <v>0</v>
@@ -1951,14 +1958,14 @@
       <c r="AS8">
         <v>0</v>
       </c>
-      <c r="AT8" s="1">
-        <v>-3.4327285982361501E-11</v>
+      <c r="AT8">
+        <v>0</v>
       </c>
       <c r="AU8" s="1">
-        <v>-1.3295010858928701E-10</v>
+        <v>-7.8676779678870597E-10</v>
       </c>
       <c r="AV8">
-        <v>46.489712965007598</v>
+        <v>56.092483562184697</v>
       </c>
       <c r="AW8">
         <v>0</v>
@@ -1970,13 +1977,13 @@
         <v>0</v>
       </c>
       <c r="AZ8">
-        <v>85068.802309189399</v>
+        <v>85056.505831859904</v>
       </c>
       <c r="BA8">
-        <v>61589.603311129002</v>
+        <v>61578.074915619698</v>
       </c>
       <c r="BB8">
-        <v>379.28550388842598</v>
+        <v>380.05358570879702</v>
       </c>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.2">
@@ -2002,19 +2009,19 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>348.574876358783</v>
+        <v>426.55068922957099</v>
       </c>
       <c r="I9">
-        <v>5958.6700849487697</v>
+        <v>6132.5855215791198</v>
       </c>
       <c r="J9">
-        <v>30565.014191755901</v>
+        <v>30492.7969034815</v>
       </c>
       <c r="K9">
-        <v>25217.5469133732</v>
+        <v>25191.975294191299</v>
       </c>
       <c r="L9">
-        <v>18557.016376922598</v>
+        <v>18499.746147696002</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -2047,10 +2054,10 @@
         <v>0.998</v>
       </c>
       <c r="W9">
-        <v>0.94699999999999995</v>
+        <v>0.93200000000000005</v>
       </c>
       <c r="X9">
-        <v>0.79900000000000004</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -2074,19 +2081,19 @@
         <v>0</v>
       </c>
       <c r="AF9">
-        <v>17428.743817939099</v>
+        <v>21327.534461478499</v>
       </c>
       <c r="AG9">
-        <v>5976.5998846025796</v>
+        <v>6151.0386374915997</v>
       </c>
       <c r="AH9">
-        <v>30626.2667252063</v>
+        <v>30553.904712907301</v>
       </c>
       <c r="AI9">
-        <v>26628.877416444899</v>
+        <v>27030.016410076401</v>
       </c>
       <c r="AJ9">
-        <v>23225.302098776701</v>
+        <v>22981.051113601399</v>
       </c>
       <c r="AK9">
         <v>0</v>
@@ -2119,13 +2126,13 @@
         <v>0</v>
       </c>
       <c r="AU9" s="1">
-        <v>-3.1338774934949201E-12</v>
+        <v>5.7919039222264902E-14</v>
       </c>
       <c r="AV9">
-        <v>10.788178300779</v>
-      </c>
-      <c r="AW9" s="1">
-        <v>-2.48717004138803E-14</v>
+        <v>122.515584251492</v>
+      </c>
+      <c r="AW9">
+        <v>0</v>
       </c>
       <c r="AX9">
         <v>0</v>
@@ -2134,13 +2141,13 @@
         <v>0</v>
       </c>
       <c r="AZ9">
-        <v>80646.822443359095</v>
+        <v>80743.654556177498</v>
       </c>
       <c r="BA9">
-        <v>57222.045606976899</v>
+        <v>57316.646779459297</v>
       </c>
       <c r="BB9">
-        <v>433.707665566819</v>
+        <v>431.47672523089102</v>
       </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.2">
@@ -2172,13 +2179,13 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1415.3489355500001</v>
+        <v>1351.9792331163201</v>
       </c>
       <c r="K10">
-        <v>36630.801228460499</v>
+        <v>36646.350538423503</v>
       </c>
       <c r="L10">
-        <v>42151.866527651298</v>
+        <v>42195.932829158497</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -2244,13 +2251,13 @@
         <v>0</v>
       </c>
       <c r="AH10">
-        <v>28884.6721540818</v>
+        <v>27591.412920741201</v>
       </c>
       <c r="AI10">
-        <v>40033.662544765597</v>
+        <v>40050.656326145901</v>
       </c>
       <c r="AJ10">
-        <v>43545.316660796801</v>
+        <v>43590.839699543903</v>
       </c>
       <c r="AK10">
         <v>0</v>
@@ -2282,11 +2289,11 @@
       <c r="AT10">
         <v>0</v>
       </c>
-      <c r="AU10" s="1">
-        <v>-4.8547826777381104E-12</v>
+      <c r="AU10">
+        <v>0</v>
       </c>
       <c r="AV10">
-        <v>10.667175412020301</v>
+        <v>1.49973408624987</v>
       </c>
       <c r="AW10">
         <v>0</v>
@@ -2298,13 +2305,13 @@
         <v>0</v>
       </c>
       <c r="AZ10">
-        <v>80198.016691661993</v>
+        <v>80194.262600697897</v>
       </c>
       <c r="BA10">
-        <v>56738.276479994602</v>
+        <v>56734.522389030899</v>
       </c>
       <c r="BB10">
-        <v>398.74429028173699</v>
+        <v>398.74429028172699</v>
       </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.2">
@@ -2339,10 +2346,10 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>2324.0690372592198</v>
+        <v>2677.0875948598</v>
       </c>
       <c r="L11">
-        <v>77889.032402131794</v>
+        <v>77551.778532794197</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -2411,10 +2418,10 @@
         <v>0</v>
       </c>
       <c r="AI11">
-        <v>28342.3053324295</v>
+        <v>32647.409693412199</v>
       </c>
       <c r="AJ11">
-        <v>77889.032402131794</v>
+        <v>77551.778532794197</v>
       </c>
       <c r="AK11">
         <v>0</v>
@@ -2449,26 +2456,26 @@
       <c r="AU11">
         <v>0</v>
       </c>
-      <c r="AV11" s="1">
-        <v>8.8424506117368198E-11</v>
-      </c>
-      <c r="AW11" s="1">
-        <v>-2.0527847732359801E-11</v>
-      </c>
-      <c r="AX11" s="1">
-        <v>-6.4184633888901396E-14</v>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+      <c r="AW11">
+        <v>0</v>
+      </c>
+      <c r="AX11">
+        <v>0</v>
       </c>
       <c r="AY11">
         <v>0</v>
       </c>
       <c r="AZ11">
-        <v>80213.101439390899</v>
+        <v>80228.866127653993</v>
       </c>
       <c r="BA11">
-        <v>56738.259512596902</v>
+        <v>56754.024200859902</v>
       </c>
       <c r="BB11">
-        <v>383.64257515503601</v>
+        <v>383.642575155072</v>
       </c>
     </row>
   </sheetData>

</xml_diff>